<commit_message>
fix lost name if you not use -t of -t > count
</commit_message>
<xml_diff>
--- a/output/google_maps_data_Unites_States_Boston_dentist
.xlsx
+++ b/output/google_maps_data_Unites_States_Boston_dentist
.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,329 +478,1515 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gypsy Place Coffee and Juice Bar</t>
+          <t>Divine Smiles</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>90 Hampshire St, Cambridge, MA 02139, États-Unis</t>
+          <t>358 Cambridge Rd, Woburn, MA 01801, United States</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>gypsyplacecoffee.com</t>
+          <t>divinesmiles.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+1 617-945-9736</t>
+          <t>+1 781-523-2558</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>280</v>
+        <v>106</v>
       </c>
       <c r="F2" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>42.3684766</v>
+        <v>42.4612521</v>
       </c>
       <c r="H2" t="n">
-        <v>-71.1667844</v>
+        <v>-71.2361195</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Boston Emergency Dental Service</t>
+          <t>Tanks-a-Lot</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>94 State St, Boston, MA 02109, États-Unis</t>
+          <t>110 School St, Everett, MA 02149, United States</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>emergencydentist247.com</t>
+          <t>tanksalotremoval.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>+1 857-227-9044</t>
+          <t>+1 617-666-0177</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="G3" t="n">
-        <v>42.3591816</v>
+        <v>42.4057217</v>
       </c>
       <c r="H3" t="n">
-        <v>-71.1273286</v>
+        <v>-71.13001800000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Boston Dental Center</t>
+          <t>Boston Dental</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>388 Commonwealth Ave B2, Boston, MA 02115, États-Unis</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>36 Chauncy St, Boston, MA 02111, United States</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>bostondental.com</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+1 617-307-7677</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+          <t>+1 617-338-5000</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>295</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.6</v>
+      </c>
       <c r="G4" t="n">
-        <v>42.3486443</v>
+        <v>42.3538708</v>
       </c>
       <c r="H4" t="n">
-        <v>-71.1621377</v>
+        <v>-71.1318071</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dental Health and Wellness Boston</t>
+          <t>Boston Dental</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>31 State St 7th Floor, Boston, MA 02109, États-Unis</t>
+          <t>35 Court St, Boston, MA 02108, United States</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dentalhealthandwellnessboston.com</t>
+          <t>bostondental.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+1 617-910-4780</t>
+          <t>+1 617-402-5000</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="F5" t="n">
         <v>4.9</v>
       </c>
       <c r="G5" t="n">
-        <v>42.3486443</v>
+        <v>42.3538708</v>
       </c>
       <c r="H5" t="n">
-        <v>-71.1621377</v>
+        <v>-71.1318071</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Boston Dental</t>
+          <t>Boston Smiles</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>36 Chauncy St, Boston, MA 02111, États-Unis</t>
+          <t>151 Merrimac St Suite 100, Boston, MA 02114, United States</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>bostondental.com</t>
+          <t>bostonsmilesdental.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+1 617-338-5000</t>
+          <t>+1 617-982-2233</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>295</v>
+        <v>242</v>
       </c>
       <c r="F6" t="n">
-        <v>4.6</v>
+        <v>4.8</v>
       </c>
       <c r="G6" t="n">
-        <v>42.3486443</v>
+        <v>42.3538708</v>
       </c>
       <c r="H6" t="n">
-        <v>-71.1621377</v>
+        <v>-71.1318071</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Boston Dental</t>
+          <t>Dental Partners of Boston - Fort Point</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>35 Court St, Boston, MA 02108, États-Unis</t>
+          <t>46 Farnsworth St, Boston, MA 02210, United States</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>bostondental.com</t>
+          <t>dentalpartnersofboston.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>+1 617-402-5000</t>
+          <t>+1 617-752-7752</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="F7" t="n">
-        <v>4.9</v>
+        <v>4.8</v>
       </c>
       <c r="G7" t="n">
-        <v>42.3486443</v>
+        <v>42.3538708</v>
       </c>
       <c r="H7" t="n">
-        <v>-71.1621377</v>
+        <v>-71.1318071</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Boston Smiles</t>
+          <t>Dental Arts of Boston</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>151 Merrimac St Suite 100, Boston, MA 02114, États-Unis</t>
+          <t>26 Marlborough St, Boston, MA 02116, United States</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>bostonsmilesdental.com</t>
+          <t>bostoncosmeticdentistma.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>+1 617-982-2233</t>
+          <t>+1 617-266-0441</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="F8" t="n">
-        <v>4.8</v>
+        <v>4.9</v>
       </c>
       <c r="G8" t="n">
-        <v>42.3486443</v>
+        <v>42.3538708</v>
       </c>
       <c r="H8" t="n">
-        <v>-71.1621377</v>
+        <v>-71.1318071</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Beacon Dental Health</t>
+          <t>New England Dental Group</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>62 On The Park, 198 Tremont St Suite 436, Boston, MA 02116, États-Unis</t>
+          <t>811 Boylston St 3rd floor, Boston, MA 02116, United States</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>beacondentalhealth.com</t>
+          <t>newenglanddentalgroup.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>+1 617-418-6940</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+          <t>+1 617-267-3993</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>347</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4.9</v>
+      </c>
       <c r="G9" t="n">
-        <v>42.3486443</v>
+        <v>42.3538708</v>
       </c>
       <c r="H9" t="n">
-        <v>-71.1621377</v>
+        <v>-71.1318071</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>New England Dental Group</t>
+          <t>Dental Associates of New England</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>811 Boylston St 3rd floor, Boston, MA 02116, États-Unis</t>
+          <t>585 Boylston St # 2, Boston, MA 02116, United States</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>newenglanddentalgroup.com</t>
+          <t>bostonsmile.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>+1 617-267-3993</t>
+          <t>+1 857-350-3400</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>345</v>
+        <v>77</v>
       </c>
       <c r="F10" t="n">
         <v>4.9</v>
       </c>
       <c r="G10" t="n">
-        <v>42.3486443</v>
+        <v>42.3538708</v>
       </c>
       <c r="H10" t="n">
-        <v>-71.1621377</v>
+        <v>-71.1318071</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Dental Arts of Boston</t>
+          <t>South Boston Dental Group</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>26 Marlborough St, Boston, MA 02116, États-Unis</t>
+          <t>29 Farragut Rd # D, Boston, MA 02127, United States</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>bostoncosmeticdentistma.com</t>
+          <t>southbostondental.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>+1 617-266-0441</t>
+          <t>+1 617-268-1030</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>189</v>
+        <v>349</v>
       </c>
       <c r="F11" t="n">
         <v>4.9</v>
       </c>
       <c r="G11" t="n">
-        <v>42.3486443</v>
+        <v>42.3538708</v>
       </c>
       <c r="H11" t="n">
-        <v>-71.1621377</v>
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Boston Dental</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>22 Boston Wharf Rd, Boston, MA 02210, United States</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>bostondental.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>+1 617-706-5000</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>101</v>
+      </c>
+      <c r="F12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Boston Premier Dentistry, PC</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10 Tremont St UNIT 402, Boston, MA 02108, United States</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>+1 617-523-2459</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>46</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CITIDental</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>63 Court St, Boston, MA 02108, United States</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>citidentalboston.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>+1 617-723-6300</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>314</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>South End Dental Arts</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>544 Tremont St, Boston, MA 02116, United States</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>southenddentalarts.com</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>+1 617-357-4943</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>26</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G15" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>East Boston Dental Associates</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>3 Meridian St, Boston, MA 02128, United States</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>+1 617-569-7300</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>161</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G16" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Faneuil Hall Dental Associates</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1 McKinley Square Lobby B, Boston, MA 02109, United States</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>fhdental.com</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>+1 617-523-4444</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>154</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5</v>
+      </c>
+      <c r="G17" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>South Boston Family Dental</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>591 E Broadway, Boston, MA 02127, United States</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>southbostonfamilydental.com</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>+1 617-268-5638</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>450</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G18" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>New England Dental Group</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1 Milk St, Boston, MA 02109, United States</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>newenglanddentalgroup.com</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>+1 617-892-4411</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>75</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G19" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Seaport Dental Associates Boston</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>451 D St #200, Boston, MA 02210, United States</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>seaportdental.com</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>+1 617-737-6453</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>260</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="G20" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Beacon Hill Dental Associates</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>77 Beacon St, Boston, MA 02108, United States</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>beaconhilldentalassociates.com</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>+1 617-523-1910</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>44</v>
+      </c>
+      <c r="F21" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G21" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Commonwealth Dental Group</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>400 Commonwealth Ave 3rd floor, Boston, MA 02215, United States</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>cdgboston.com</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>+1 617-266-8770</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>135</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G22" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mass Dental Associates</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1313 Washington St, Boston, MA 02118, United States</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>massdentalassociates.net</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>+1 617-859-3939</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>122</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G23" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Commonwealth Dental Group</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>400 Commonwealth Ave 3rd floor, Boston, MA 02215, United States</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>cdgboston.com</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>+1 617-266-8770</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>135</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G24" t="n">
+        <v>42.3538708</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-71.1318071</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Great Hill Dental - Boston</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1610 Tremont St, Boston, MA 02120, United States</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>boston.greathilldental.com</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>+1 617-379-1966</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>427</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G25" t="n">
+        <v>42.3337321</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-71.176046</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Dental Partners of Boston at Prudential Center</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>800 Boylston St 2nd floor, Boston, MA 02199, United States</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>dentalpartnersofboston.com</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>+1 617-829-9744</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>309</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G26" t="n">
+        <v>42.3337321</v>
+      </c>
+      <c r="H26" t="n">
+        <v>-71.176046</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Mass Dental Associates</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1313 Washington St, Boston, MA 02118, United States</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>massdentalassociates.net</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>+1 617-859-3939</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>122</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G27" t="n">
+        <v>42.3337321</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-71.176046</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Gentle Dental South Boston</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>368A W Broadway, Boston, MA 02127, United States</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>gentledental.com</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>+1 617-934-2469</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>218</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G28" t="n">
+        <v>42.3378589</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-71.1212204</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>AP Dental Center</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>231 Border St B, Boston, MA 02128, United States</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>apdentalcenter.com</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>+1 617-315-1515</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>306</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G29" t="n">
+        <v>42.3378589</v>
+      </c>
+      <c r="H29" t="n">
+        <v>-71.1212204</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Dental Partners of Boston at Charles River</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>50 Staniford St #303, Boston, MA 02114, United States</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>dentalpartnersofboston.com</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>+1 617-812-2071</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>171</v>
+      </c>
+      <c r="F30" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G30" t="n">
+        <v>42.3378589</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-71.1212204</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Beacon Hill Dental Associates</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>77 Beacon St, Boston, MA 02108, United States</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>beaconhilldentalassociates.com</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>+1 617-523-1910</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>44</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G31" t="n">
+        <v>42.3378589</v>
+      </c>
+      <c r="H31" t="n">
+        <v>-71.1212204</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Ace Dental Boston- Hyde Park</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1138 River St, Boston, MA 02136, United States</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>acedentalboston.com</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>+1 617-361-5020</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>1035</v>
+      </c>
+      <c r="F32" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="G32" t="n">
+        <v>42.257002</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-71.192009</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Dr. Dental: Dentistry &amp; Braces</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>45 Maverick Square, East Boston, MA 02128, United States</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>mydrdental.com</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>+1 617-567-3800</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>454</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G33" t="n">
+        <v>42.3694004</v>
+      </c>
+      <c r="H33" t="n">
+        <v>-71.1109755</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Back Bay Dental Associates</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>745 Boylston St Suite 206, Boston, MA 02116, United States</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>backbaydental.doctormmdev2.com</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>+1 617-536-4545</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>18</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G34" t="n">
+        <v>42.349494</v>
+      </c>
+      <c r="H34" t="n">
+        <v>-71.1527182</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CITIDental South Boston</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>141 Dorchester Ave, Boston, MA 02127, United States</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>citidentalsouthboston.com</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>+1 617-482-7300</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>162</v>
+      </c>
+      <c r="F35" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G35" t="n">
+        <v>42.349494</v>
+      </c>
+      <c r="H35" t="n">
+        <v>-71.1527182</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>East Boston Family Dental Center: Rahmatpour Mehdi DDS</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>79 Meridian St, Boston, MA 02128, United States</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>+1 617-567-8882</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>20</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G36" t="n">
+        <v>42.3722821</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-71.1109191</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Boston Teeth Associates</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>359 Boylston St, Boston, MA 02116, United States</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>bostonteeth.com</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>+1 617-262-1422</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>5</v>
+      </c>
+      <c r="F37" t="n">
+        <v>5</v>
+      </c>
+      <c r="G37" t="n">
+        <v>42.3519619</v>
+      </c>
+      <c r="H37" t="n">
+        <v>-71.1437165</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Devonshire Dental of Boston</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>185 Devonshire St STE 410, Boston, MA 02110, United States</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>devonshiredental.net</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>+1 617-350-7474</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>483</v>
+      </c>
+      <c r="F38" t="n">
+        <v>5</v>
+      </c>
+      <c r="G38" t="n">
+        <v>42.3519619</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-71.1437165</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Dental Care at South Boston Community Health Center</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Dental Department, 386 W Broadway, Boston, MA 02127, United States</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>sbchc.org</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>+1 617-464-5825</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>9</v>
+      </c>
+      <c r="F39" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>42.3519619</v>
+      </c>
+      <c r="H39" t="n">
+        <v>-71.1437165</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Dr. Dental: Dentistry &amp; Braces</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>55 Meridian St, East Boston, MA 02128, United States</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>mydrdental.com</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>+1 617-567-1300</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>400</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G40" t="n">
+        <v>42.3519619</v>
+      </c>
+      <c r="H40" t="n">
+        <v>-71.1437165</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Boston University Henry M. Goldman School of Dental Medicine</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>635 Albany St, Boston, MA 02118, United States</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>bu.edu</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>+1 617-358-8300</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>143</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="G41" t="n">
+        <v>42.3519619</v>
+      </c>
+      <c r="H41" t="n">
+        <v>-71.1437165</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Emergency Dentist Boston</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>140 Havre St, Boston, MA 02128, United States</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>emergencydentist247.com</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>+1 617-765-9691</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4</v>
+      </c>
+      <c r="G42" t="n">
+        <v>42.3768269</v>
+      </c>
+      <c r="H42" t="n">
+        <v>-71.1061699</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>West Broadway Family Dental</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>385 W Broadway, South Boston, MA 02127, United States</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>wbfamilydental.com</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>+1 617-268-8242</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>260</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G43" t="n">
+        <v>42.3768269</v>
+      </c>
+      <c r="H43" t="n">
+        <v>-71.1061699</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Dental Esthetics Boston</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>dentalestheticsboston.com</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>+1 617-536-3054</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" t="n">
+        <v>5</v>
+      </c>
+      <c r="G44" t="n">
+        <v>42.31435</v>
+      </c>
+      <c r="H44" t="n">
+        <v>-71.0423818</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Unity Dental</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>4172 Washington St, Roslindale, MA 02131, United States</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>myunitydental.com</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>+1 617-313-7123</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>107</v>
+      </c>
+      <c r="F45" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="G45" t="n">
+        <v>42.2877104</v>
+      </c>
+      <c r="H45" t="n">
+        <v>-71.1987151</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>My Dental - East Boston</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>151 Meridian St, East Boston, MA 02128, United States</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>mydentalcares.com</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>+1 857-322-1011</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>26</v>
+      </c>
+      <c r="F46" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G46" t="n">
+        <v>42.3737997</v>
+      </c>
+      <c r="H46" t="n">
+        <v>-71.11100260000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>